<commit_message>
mend zyj time manage excle
</commit_message>
<xml_diff>
--- a/documents/TimeManage_ZYJ.xlsx
+++ b/documents/TimeManage_ZYJ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="9795"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>日期</t>
   </si>
@@ -69,6 +69,14 @@
     <t>球的血量现在是以颜色辨别。
 为了不让颜色太多而使人眼花，
 现在暂定有5种颜色。</t>
+  </si>
+  <si>
+    <t>2012.4.10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习git相关操作，对git的分支操作有了更多的了解。上传git搭建和使用文档</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -438,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -517,6 +525,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="27">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new game ifno by zhaoyj
</commit_message>
<xml_diff>
--- a/documents/TimeManage_ZYJ.xlsx
+++ b/documents/TimeManage_ZYJ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="21015" windowHeight="8955"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="20940" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>日期</t>
   </si>
@@ -76,6 +76,14 @@
   </si>
   <si>
     <t>学习git相关操作，对git的分支操作有了更多的了解。上传git搭建和使用文档</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计游戏《可爱糖果对对碰》思路，并上传</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -446,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -536,6 +544,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>